<commit_message>
update the location point coordinate
</commit_message>
<xml_diff>
--- a/_ref/POI_MAP.xlsx
+++ b/_ref/POI_MAP.xlsx
@@ -512,7 +512,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>22.414361</v>
+        <v>22.414670000000001</v>
       </c>
       <c r="E2">
         <v>114.210292</v>
@@ -582,10 +582,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>22.417777999999998</v>
+        <v>22.417739999999998</v>
       </c>
       <c r="E3">
-        <v>114.210284</v>
+        <v>114.210734</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -605,10 +605,10 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>22.417793</v>
+        <v>22.417773</v>
       </c>
       <c r="E4">
-        <v>114.21129000000001</v>
+        <v>114.21135</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -628,10 +628,10 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>22.419737000000001</v>
+        <v>22.419830000000001</v>
       </c>
       <c r="E5">
-        <v>114.206974</v>
+        <v>114.207024</v>
       </c>
       <c r="F5">
         <v>50</v>
@@ -651,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>22.419784</v>
+        <v>22.41986</v>
       </c>
       <c r="E6">
-        <v>114.203401</v>
+        <v>114.20327</v>
       </c>
       <c r="F6">
         <v>50</v>
@@ -674,10 +674,10 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>22.420463000000002</v>
+        <v>22.420362999999998</v>
       </c>
       <c r="E7">
-        <v>114.20531099999999</v>
+        <v>114.20518</v>
       </c>
       <c r="F7">
         <v>50</v>
@@ -720,10 +720,10 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>22.418662999999999</v>
+        <v>22.418780000000002</v>
       </c>
       <c r="E9">
-        <v>114.20528400000001</v>
+        <v>114.20526</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -743,10 +743,10 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>22.418358000000001</v>
+        <v>22.418520000000001</v>
       </c>
       <c r="E10">
-        <v>114.209289</v>
+        <v>114.20874999999999</v>
       </c>
       <c r="F10">
         <v>30</v>
@@ -766,10 +766,10 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>22.421603999999999</v>
+        <v>22.421340000000001</v>
       </c>
       <c r="E11">
-        <v>114.203136</v>
+        <v>114.20345</v>
       </c>
       <c r="F11">
         <v>30</v>
@@ -881,10 +881,10 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>22.421966000000001</v>
+        <v>22.421849999999999</v>
       </c>
       <c r="E16">
-        <v>114.20494600000001</v>
+        <v>114.2046</v>
       </c>
       <c r="F16">
         <v>30</v>
@@ -904,10 +904,10 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>22.420002</v>
+        <v>22.420359999999999</v>
       </c>
       <c r="E17">
-        <v>114.212384</v>
+        <v>114.2122</v>
       </c>
       <c r="F17">
         <v>40</v>
@@ -927,10 +927,10 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>22.415306000000001</v>
+        <v>22.415541000000001</v>
       </c>
       <c r="E18">
-        <v>114.208428</v>
+        <v>114.208218</v>
       </c>
       <c r="F18">
         <v>50</v>
@@ -950,7 +950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>